<commit_message>
Added run.bat file and plugin (maven-compiler and surefireplugin)
Added run.bat file and plugin (maven-compiler and surefireplugin)
</commit_message>
<xml_diff>
--- a/nordson.omu/src/test/java/com/nordson/testData/LoginData.xlsx
+++ b/nordson.omu/src/test/java/com/nordson/testData/LoginData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SOURCEBITS -NORDSON PROJECT\nordson.omu\src\test\java\com\nordson\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ravi Raj\git\nordsonomu_automation\nordson.omu\src\test\java\com\nordson\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E765273-06FD-4C69-B540-1B03AFE0B342}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2098D84B-E624-47EA-A4AF-DF0EA045D18C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{0DCA89EA-4F37-48B5-B8D2-472A325DFB74}"/>
+    <workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{0DCA89EA-4F37-48B5-B8D2-472A325DFB74}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -513,7 +513,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.21875" customWidth="1"/>
+    <col min="1" max="1" width="29.21875" customWidth="1"/>
     <col min="2" max="2" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -530,7 +530,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>12345678</v>
+        <v>123456789</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new Changes to HTML Reports
</commit_message>
<xml_diff>
--- a/nordson.omu/src/test/java/com/nordson/testData/LoginData.xlsx
+++ b/nordson.omu/src/test/java/com/nordson/testData/LoginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ravi Raj\git\nordsonomu_automation\nordson.omu\src\test\java\com\nordson\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2098D84B-E624-47EA-A4AF-DF0EA045D18C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB8F54F-F34C-4D96-B961-2EED83AF17F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{0DCA89EA-4F37-48B5-B8D2-472A325DFB74}"/>
   </bookViews>
@@ -508,7 +508,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -530,7 +530,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>123456789</v>
+        <v>12345678</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
POC1 and POC2 commit
Added new file TC_Pressure_Min_Max_Data_Validations
</commit_message>
<xml_diff>
--- a/nordson.omu/src/test/java/com/nordson/testData/LoginData.xlsx
+++ b/nordson.omu/src/test/java/com/nordson/testData/LoginData.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ravi Raj\git\nordsonomu_automation\nordson.omu\src\test\java\com\nordson\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB8F54F-F34C-4D96-B961-2EED83AF17F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE592F09-E700-4B12-BB09-CD76D4400E0E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{0DCA89EA-4F37-48B5-B8D2-472A325DFB74}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0DCA89EA-4F37-48B5-B8D2-472A325DFB74}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="LinksLogin" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,18 +34,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>Password</t>
   </si>
   <si>
     <t>UserName</t>
-  </si>
-  <si>
-    <t>amrendrasadmin@yopmail.com</t>
-  </si>
-  <si>
-    <t>pass1234</t>
   </si>
   <si>
     <t>raviuser@yopmail.com</t>
@@ -55,7 +49,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,14 +76,6 @@
       <b/>
       <sz val="11"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color indexed="30"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -147,10 +133,10 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel Built-in Normal" xfId="2" xr:uid="{19DFC39A-23B0-4ADC-AB54-D047D0C5623A}"/>
@@ -469,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8E1DBC9-FCF4-45E5-B4FD-5A6169F6B019}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -488,11 +474,11 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>3</v>
+      <c r="B2" s="2">
+        <v>12345678</v>
       </c>
     </row>
   </sheetData>
@@ -507,8 +493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6450C58C-0634-4148-B924-699D95376F3E}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -518,16 +504,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>12345678</v>
@@ -538,5 +524,6 @@
     <hyperlink ref="A2" r:id="rId1" xr:uid="{71FEE756-8C55-41BC-B865-A20D4B8D72C6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
POC- Retrive Values from MDS File for Temperature
</commit_message>
<xml_diff>
--- a/nordson.omu/src/test/java/com/nordson/testData/LoginData.xlsx
+++ b/nordson.omu/src/test/java/com/nordson/testData/LoginData.xlsx
@@ -1,33 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ravi Raj\git\nordsonomu_automation\nordson.omu\src\test\java\com\nordson\testData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB8F54F-F34C-4D96-B961-2EED83AF17F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{2EF05ACD-A67C-471B-B8E2-2903BFB1F628}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{0DCA89EA-4F37-48B5-B8D2-472A325DFB74}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17328" windowHeight="13224" xr2:uid="{0DCA89EA-4F37-48B5-B8D2-472A325DFB74}"/>
   </bookViews>
   <sheets>
-    <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="LinksLogin" sheetId="2" r:id="rId2"/>
+    <sheet name="Login" sheetId="2" r:id="rId1"/>
+    <sheet name="AdminLogin" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <oleSize ref="A1:P24"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -466,11 +454,49 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6450C58C-0634-4148-B924-699D95376F3E}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="29.21875" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>12345678</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{71FEE756-8C55-41BC-B865-A20D4B8D72C6}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8E1DBC9-FCF4-45E5-B4FD-5A6169F6B019}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD20"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -501,42 +527,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6450C58C-0634-4148-B924-699D95376F3E}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="29.21875" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2">
-        <v>12345678</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{71FEE756-8C55-41BC-B865-A20D4B8D72C6}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
commit new changes jira ticket
</commit_message>
<xml_diff>
--- a/nordson.omu/src/test/java/com/nordson/testData/LoginData.xlsx
+++ b/nordson.omu/src/test/java/com/nordson/testData/LoginData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\New_Nordosn_Work\nordsonomu_automation\nordson.omu\src\test\java\com\nordson\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{379FCAE8-59EE-4B37-8A20-76A25E09EDF1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC09744-CF51-4C02-80FF-004DEA783277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{0DCA89EA-4F37-48B5-B8D2-472A325DFB74}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0DCA89EA-4F37-48B5-B8D2-472A325DFB74}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="2" r:id="rId1"/>
@@ -41,10 +41,10 @@
     <t>pass1234</t>
   </si>
   <si>
-    <t>raviuser@yopmail.com</t>
+    <t>autouser4@yopmail.com</t>
   </si>
   <si>
-    <t>autouser4@yopmail.com</t>
+    <t>raviuser@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -465,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6450C58C-0634-4148-B924-699D95376F3E}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -485,10 +485,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2">
-        <v>12345678</v>
+        <v>123456789</v>
       </c>
     </row>
   </sheetData>
@@ -541,7 +541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B86030FE-F38A-4D5B-A289-B31333643154}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
@@ -561,7 +561,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>12345678</v>

</xml_diff>